<commit_message>
add user input example
</commit_message>
<xml_diff>
--- a/extra/questions.xlsx
+++ b/extra/questions.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">2 + 1?</t>
   </si>
   <si>
-    <t xml:space="preserve">dio esiste?</t>
+    <t xml:space="preserve">dio esiste</t>
   </si>
   <si>
     <t xml:space="preserve">si</t>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">no</t>
   </si>
   <si>
-    <t xml:space="preserve">2 + 2?</t>
+    <t xml:space="preserve">4 + 5?</t>
   </si>
   <si>
     <t xml:space="preserve">…</t>
@@ -157,13 +157,13 @@
   <dimension ref="A1:AMJ4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="8.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="8.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="9.47"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
@@ -232,7 +232,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>8</v>

</xml_diff>